<commit_message>
Added possible terms in annotation spreadsheet
</commit_message>
<xml_diff>
--- a/productionplanning/doc/pps-term-annotation-v1.0.xlsx
+++ b/productionplanning/doc/pps-term-annotation-v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arkop\git\iofoundry\ontology-pps_branch\productionplanning\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6AD62C-BDEA-4B2C-82FA-D7F994524EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2741188-0982-4143-9FA4-1C42A40BB5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C372C5C8-D15D-498D-A330-70E8AF16022C}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="120">
   <si>
     <t>Comment</t>
   </si>
@@ -247,13 +247,208 @@
   </si>
   <si>
     <t>plan that aims at producing a product as specified or fulfill some production order</t>
+  </si>
+  <si>
+    <t>ProcessPlan</t>
+  </si>
+  <si>
+    <t>process plan</t>
+  </si>
+  <si>
+    <t>StepSpecification</t>
+  </si>
+  <si>
+    <t>PlanDocument</t>
+  </si>
+  <si>
+    <t>ProductSpecification</t>
+  </si>
+  <si>
+    <t>ProductionOrderSpecification</t>
+  </si>
+  <si>
+    <t>CooccurringStepSpecification</t>
+  </si>
+  <si>
+    <t>PrecedingStepSpecification</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>MaterialStateDescription</t>
+  </si>
+  <si>
+    <t>MaterialFlowDescription</t>
+  </si>
+  <si>
+    <t>ControlFlowDescription</t>
+  </si>
+  <si>
+    <t>MaterialFlow</t>
+  </si>
+  <si>
+    <t>ControlFlow</t>
+  </si>
+  <si>
+    <t>ResourceDescription</t>
+  </si>
+  <si>
+    <t>hasSubProcessPlan</t>
+  </si>
+  <si>
+    <t>hasSpecifiedStep</t>
+  </si>
+  <si>
+    <t>hasAssociatedStep</t>
+  </si>
+  <si>
+    <t>hasSpecifiedResource</t>
+  </si>
+  <si>
+    <t>hasSpecifiedOutput</t>
+  </si>
+  <si>
+    <t>hasSpecifiedInput</t>
+  </si>
+  <si>
+    <t>PlanningProcess</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>MachinedFeatureSpecification</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>SchedulingProcess</t>
+  </si>
+  <si>
+    <t>AssemblySpecification</t>
+  </si>
+  <si>
+    <t>ProductDesign</t>
+  </si>
+  <si>
+    <t>WorkStation</t>
+  </si>
+  <si>
+    <t>ManufacturingCell</t>
+  </si>
+  <si>
+    <t>Buffer</t>
+  </si>
+  <si>
+    <t>Allocation</t>
+  </si>
+  <si>
+    <t>PlanningHorizon</t>
+  </si>
+  <si>
+    <t>FlowShop</t>
+  </si>
+  <si>
+    <t>Line, Assembly Line</t>
+  </si>
+  <si>
+    <t>JobShop</t>
+  </si>
+  <si>
+    <t>AssemblyFeatureSpecification</t>
+  </si>
+  <si>
+    <t>FeatureSpecification</t>
+  </si>
+  <si>
+    <t>ConsumableResource</t>
+  </si>
+  <si>
+    <t>Task, Action</t>
+  </si>
+  <si>
+    <t>Lot</t>
+  </si>
+  <si>
+    <t>Preemption</t>
+  </si>
+  <si>
+    <t>OrderQuantity</t>
+  </si>
+  <si>
+    <t>SchedulingPerformanceMeasure</t>
+  </si>
+  <si>
+    <t>CompletionTime</t>
+  </si>
+  <si>
+    <t>FlowTime</t>
+  </si>
+  <si>
+    <t>Lateness</t>
+  </si>
+  <si>
+    <t>ProcessingTime</t>
+  </si>
+  <si>
+    <t>DueDate</t>
+  </si>
+  <si>
+    <t>ReleaseDate</t>
+  </si>
+  <si>
+    <t>Tardiness</t>
+  </si>
+  <si>
+    <t>Earliness</t>
+  </si>
+  <si>
+    <t>TotalCompletionTime</t>
+  </si>
+  <si>
+    <t>AverageCompletionTime</t>
+  </si>
+  <si>
+    <t>TotalFlowTime</t>
+  </si>
+  <si>
+    <t>AverageFlowTime</t>
+  </si>
+  <si>
+    <t>TotalLateness</t>
+  </si>
+  <si>
+    <t>AverageLateness</t>
+  </si>
+  <si>
+    <t>NumberOfTardyJobs</t>
+  </si>
+  <si>
+    <t>AverageNumberOfTardyJob</t>
+  </si>
+  <si>
+    <t>NumberOfEarlyJob</t>
+  </si>
+  <si>
+    <t>AverageNumberOfEarlyJob</t>
+  </si>
+  <si>
+    <t>TotalEarliness</t>
+  </si>
+  <si>
+    <t>AverageEarliness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,25 +464,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -308,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -323,12 +506,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -673,18 +853,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4609C435-C663-43F5-B15B-8E0DF516E28E}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Y61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
+      <selection pane="bottomRight" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.77734375" style="4" customWidth="1"/>
     <col min="2" max="2" width="23.44140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="16" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -707,193 +887,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="b">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="6" t="b">
+      <c r="J2" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="7" t="s">
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6" t="s">
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
     </row>
     <row r="3" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="6" t="b">
+      <c r="I3" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="J3" s="6" t="b">
+      <c r="J3" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6" t="s">
+      <c r="K3" s="5"/>
+      <c r="L3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6" t="s">
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="6"/>
+      <c r="X3" s="5"/>
     </row>
     <row r="4" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -919,6 +1099,303 @@
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="X4" s="3"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -941,15 +1418,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACAF60D7-9FD2-4302-A96C-94B975648674}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21" style="1" customWidth="1"/>
     <col min="2" max="5" width="38" style="1" customWidth="1"/>
     <col min="6" max="6" width="30.6640625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.6640625" style="1"/>
@@ -977,21 +1454,43 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="A5" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>